<commit_message>
Updated lammps lj graph to fix y-axis. Fixed webiste bibliographies to be consistant and conforming to bibtex website citation standards
</commit_message>
<xml_diff>
--- a/lammps_kvm_scale_updated.xlsx
+++ b/lammps_kvm_scale_updated.xlsx
@@ -1120,14 +1120,7 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout>
-            <c:manualLayout>
-              <c:xMode val="edge"/>
-              <c:yMode val="edge"/>
-              <c:x val="1.1715175487794079E-2"/>
-              <c:y val="0.28264535795838741"/>
-            </c:manualLayout>
-          </c:layout>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -3311,7 +3304,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="204" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="169" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>